<commit_message>
aggiornamento DHW e schedules
</commit_message>
<xml_diff>
--- a/eureca_ubem/Input/systems.xlsx
+++ b/eureca_ubem/Input/systems.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pratenr82256\Desktop\EUReCA\eureca_ubem\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\borgnic12709\Desktop\eureca_2\EUReCA\eureca_ubem\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD67A0C2-DF03-4E39-8AB6-3849FC15012C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D1BDDB-D7F1-415C-A9E5-C3D6724C9460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1890" windowWidth="29040" windowHeight="16440" xr2:uid="{40FA4DE4-75D5-41EF-A942-92EA28EAAAE1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{40FA4DE4-75D5-41EF-A942-92EA28EAAAE1}"/>
   </bookViews>
   <sheets>
     <sheet name="HeatingSystems" sheetId="1" r:id="rId1"/>
@@ -44,10 +44,10 @@
   <commentList>
     <comment ref="J1" authorId="0" shapeId="0" xr:uid="{54E47AA3-69A9-491B-B19F-86EC83837327}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    If system is HP this should be set every time, otherwise the code will consider a 1 default value</t>
+        <t>[Commento in thread]
+La versione di Excel in uso consente di leggere questo commento in thread, ma tutte le modifiche a esso apportate verranno rimosse se il file viene aperto in una versione più recente di Excel. Ulteriori informazioni: https://go.microsoft.com/fwlink/?linkid=870924
+Commento:
+If system is HP this should be set every time, otherwise the code will consider a 1 default value</t>
       </text>
     </comment>
   </commentList>
@@ -445,7 +445,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -467,7 +467,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -793,21 +793,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AA04150-DEC4-4810-9D83-7EA066A33DD0}">
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="33.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" style="1" customWidth="1"/>
     <col min="4" max="12" width="13" style="1" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" customWidth="1"/>
-    <col min="14" max="16" width="13.5703125" customWidth="1"/>
+    <col min="13" max="13" width="13.44140625" customWidth="1"/>
+    <col min="14" max="16" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -860,7 +860,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -908,7 +908,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -956,7 +956,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>81</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>82</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>83</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>84</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>85</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>86</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>87</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>88</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>89</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>90</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>91</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>92</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>93</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>94</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>95</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>96</v>
       </c>
@@ -1932,7 +1932,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>97</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>98</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>99</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>100</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>101</v>
       </c>
@@ -2162,7 +2162,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>102</v>
       </c>
@@ -2208,7 +2208,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>103</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>104</v>
       </c>
@@ -2300,7 +2300,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>105</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>106</v>
       </c>
@@ -2395,7 +2395,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>107</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>108</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>109</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>110</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>111</v>
       </c>
@@ -2650,7 +2650,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>112</v>
       </c>
@@ -2707,15 +2707,15 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="10" width="18.42578125" customWidth="1"/>
+    <col min="1" max="10" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2747,7 +2747,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -2802,7 +2802,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>26</v>
       </c>

</xml_diff>